<commit_message>
filled in the missing age values
</commit_message>
<xml_diff>
--- a/Data/raw_imaging_data.xlsx
+++ b/Data/raw_imaging_data.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonahschwartz/Documents/GitHub/Projects/ent-imaging-analysis/Data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/jonahschwartz/Documents/GitHub/Sleep-Final-Project/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{323512C4-4E17-5A4B-9CCD-78C8DBF94931}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8EF41F91-3F89-B642-BD89-3179B3FA59FB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="1280" windowWidth="28800" windowHeight="16440" xr2:uid="{9C7DD11A-90AC-4141-B5D8-9465E75F7745}"/>
+    <workbookView xWindow="0" yWindow="520" windowWidth="28800" windowHeight="16460" xr2:uid="{9C7DD11A-90AC-4141-B5D8-9465E75F7745}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -586,8 +586,8 @@
   <dimension ref="A1:K406"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A223" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E226" sqref="E226"/>
+      <pane ySplit="1" topLeftCell="A83" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="E119" sqref="E119"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -6107,6 +6107,9 @@
       <c r="B158" s="2">
         <v>212628</v>
       </c>
+      <c r="C158" s="2">
+        <v>74</v>
+      </c>
       <c r="D158" s="2" t="s">
         <v>5</v>
       </c>
@@ -9008,6 +9011,9 @@
       </c>
       <c r="B241" s="2">
         <v>281633</v>
+      </c>
+      <c r="C241" s="2">
+        <v>58</v>
       </c>
       <c r="D241" s="2" t="s">
         <v>5</v>

</xml_diff>